<commit_message>
all activity tests updated to run with the new UI
</commit_message>
<xml_diff>
--- a/matthew.fuller/results.xlsx
+++ b/matthew.fuller/results.xlsx
@@ -16,264 +16,158 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
   <si>
     <t>NAMES</t>
   </si>
   <si>
     <t>ÿþ Running tests in
- - Chrome 9204515159  Windows 10
+ - Chrome 930457782  Windows 10
  activity tests
  ê</t>
   </si>
   <si>
     <t xml:space="preserve"> can open activity creation menu
  - DEPRECATED can navigate to test from feed page
+ ê</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> can navigate to edit activity
+ ê</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> can create an activity
+ - DEPRECATED can edit activity title 
+ ê</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> can create an activity with multiple groups
  </t>
   </si>
   <si>
-    <t xml:space="preserve"> can navigate to edit activity
+    <t xml:space="preserve"> edit title of activity
+ ê</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> edit description of activity
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cannot create an activity without a title or desc
    1) AssertionError expected false to deeply equal true
       + expected - actual
       -false
       +true
-      Browser Chrome 9204515159  Windows 10
-         175 áááá   checking if activity title exists
-         176   returns null
-         177 
-         178 async pressCreateBtn() 
-         179   await t
-        180     expect(thiscreateBtnexists)eql(true)
-         181     click(thiscreateBtn)
-         182     wait(2000)
-         183     expect(Selector(activityTitle)exists)
-         184     eql(true)
-         185   return null
+      Browser Chrome 930457782  Windows 10
+         125   await activitiesaddEndData()
+         126   await t
+         127     expect(activitiescreateBtnexists)eql(true)
+         128     click(activitiescreateBtn)
+         129 
+      expect(Selector(spanerrorcreateButtonstopactive)exists)
+        130     eql(true)
+         131 )
+         132  description attempt to create an activity without
+      fillign any fields in 
+         133 test(cannot create an activity without any info async (t)
+         134   await feedPageopenCreateMenu()
+         135   await activitiesclickCreateActivity()
+         at anonymous
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs1306)
+         at fulfilled
+      (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs558)
+ </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> cannot create an activity without any info
+   1) The specified selector does not match any element in the DOM tree
+      á  Selector(adropdown-item)
+      á     withAttribute(data-title Activity)
+      Browser Chrome 930457782  Windows 10
+         82 áááá
+         83 
+         84 async clickCreateActivity() 
+         85   await t
+         86     setNativeDialogHandler(()  true)
+        87     click(feedPagecreateOptionsActivity)
+         88     expect(thisactivitiesSearchBatexists)eql(true)
+         89 
+         90 
+         91  description in the activities creation menu click on to
+      the calender and then select a day 
+         92 async clickOnDayInCurrentMonth(daystring) 
          at ActivityPageanonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets18037)
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets877)
+         at anonymous
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets871)
+         at __awaiter
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets412)
+         at ActivityPageclickCreateActivity
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets6516)
+         at anonymous
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs13520)
+         at fulfilled
+      (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs558)
+ ê</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> edit endDate of activity
+   1) AssertionError expected false to deeply equal true
+      + expected - actual
+      -false
+      +true
+      Browser Chrome 930457782  Windows 10
+         215 áááá  await t
+         216     expect(thiscreateBtnexists)eql(true)
+         217     click(thiscreateBtn)
+         218     wait(2000)
+         219     expect(Selector(divappTitle)child(span)exists)
+        220     eql(true)
+         221   return null
+         222 
+         223 
+         224 async addGenericTitleAndDescription(useObj  false obj 
+      new ActivityObj()) 
+         225   let title
+         at ActivityPageanonymous
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets2207)
          at anonymous
    (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets871)
          at __awaiter
    (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets412)
          at ActivityPagepressCreateBtn
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets16916)
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets20116)
          at ActivityPageanonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets8715)
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets19015)
          at fulfilled
       (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets558)
  </t>
   </si>
   <si>
-    <t xml:space="preserve"> can create an activity
+    <t xml:space="preserve"> edit startDate of activity
    1) AssertionError expected false to deeply equal true
       + expected - actual
       -false
       +true
-      Browser Chrome 9204515159  Windows 10
-         63 test(can create an activity async (t)  
-         64   await feedPageopenCreateMenu()
-         65   await t
-         66     setNativeDialogHandler(()  true)
-         67     click(feedPagecreateOptionsActivity)
-        68 
-      expect(Selector(search-tab-tab-Content)exists)eql(true)
-         69   await activitiesaddEndData()
-         70   await activitiesaddNthGroup(0)
-         71   await activitiespressCreateBtn()
-         72 )
-         73  deprecated replaced with cleaner test 
-         at anonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs6857)
-         at fulfilled
-      (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs558)
- - DEPRECATED can edit activity title 
- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> can create an activity with multiple groups
-   1) AssertionError expected false to deeply equal true
-      + expected - actual
-      -false
-      +true
-      Browser Chrome 9204515159  Windows 10
-         101 test(can create an activity with multiple groups async
-      (t)  
-         102   await feedPageopenCreateMenu()
-         103   await t
-         104     setNativeDialogHandler(()  true)
-         105     click(feedPagecreateOptionsActivity)
-        106 
-      expect(Selector(search-tab-tab-Content)exists)eql(true)
-         107   await activitiesaddEndData()
-         108   await activitiesaddNthGroup(0)
-         109   await activitiesaddNthGroup(1)
-         110   await activitiesaddNthGroup(2)
-         111   await activitiesaddGenericTitleAndDescription()
-         at anonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs10657)
-         at fulfilled
-      (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs558)
- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cannot create an activity without a title or desc
-   1) AssertionError expected false to deeply equal true
-      + expected - actual
-      -false
-      +true
-      Browser Chrome 9204515159  Windows 10
-         131 test(cannot create an activity without a title or desc
-      async (t)  
-         132   await feedPageopenCreateMenu()
-         133   await t
-         134     setNativeDialogHandler(()  true)
-         135     click(feedPagecreateOptionsActivity)
-        136 
-      expect(Selector(search-tab-tab-Content)exists)eql(true)
-         137   await activitiesaddNthGroup(0)
-         138   await activitiesaddEndData()
-         139   await t
-         140     expect(activitiescreateBtnexists)eql(true)
-         141     click(activitiescreateBtn)
-         at anonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs13657)
-         at fulfilled
-      (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs558)
- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> cannot create an activity without any info
-   1) AssertionError expected false to deeply equal true
-      + expected - actual
-      -false
-      +true
-      Browser Chrome 9204515159  Windows 10
-         146 test(cannot create an activity without any info async (t)
-         147   await feedPageopenCreateMenu()
-         148   await t
-         149     setNativeDialogHandler(()  true)
-         150     click(feedPagecreateOptionsActivity)
-        151 
-      expect(Selector(search-tab-tab-Content)exists)eql(true)
-         152   await t
-         153     expect(activitiescreateBtnexists)eql(true)
-         154     click(activitiescreateBtn)
-         155 
-      expect(Selector(spanerrorcreateButtonstopactive)exists)
-         156     eql(true)
-         at anonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs15157)
-         at fulfilled
-      (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerTestsactivity-teststs558)
- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> edit title of activity
-   1) AssertionError expected false to deeply equal true
-      + expected - actual
-      -false
-      +true
-      Browser Chrome 9204515159  Windows 10
-         175 áááá   checking if activity title exists
-         176   returns null
-         177 
-         178 async pressCreateBtn() 
-         179   await t
-        180     expect(thiscreateBtnexists)eql(true)
-         181     click(thiscreateBtn)
-         182     wait(2000)
-         183     expect(Selector(activityTitle)exists)
-         184     eql(true)
-         185   return null
+      Browser Chrome 930457782  Windows 10
+         201 áááá  const test  await String(inntrText)toUpperCase()
+         202    consolelog(inner +test)
+         203    consolelog(inner +inntrText)
+         204    consolelog(text +text)
+         205    set both to uppercase to account for differences
+        206   await texpect(test  texttoUpperCase())eql(true)
+         207 
+         208 
+         209 
+         210   description press the create button of a activity and
+      verify its creation by
+         211    checking if activity title exists
          at ActivityPageanonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets18037)
-         at anonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets871)
-         at __awaiter
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets412)
-         at ActivityPagepressCreateBtn
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets16916)
-         at ActivityPageanonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets8715)
+   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets20648)
          at fulfilled
       (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets558)
- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> edit description of activity
-   1) AssertionError expected false to deeply equal true
-      + expected - actual
-      -false
-      +true
-      Browser Chrome 9204515159  Windows 10
-         175 áááá   checking if activity title exists
-         176   returns null
-         177 
-         178 async pressCreateBtn() 
-         179   await t
-        180     expect(thiscreateBtnexists)eql(true)
-         181     click(thiscreateBtn)
-         182     wait(2000)
-         183     expect(Selector(activityTitle)exists)
-         184     eql(true)
-         185   return null
-         at ActivityPageanonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets18037)
-         at anonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets871)
-         at __awaiter
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets412)
-         at ActivityPagepressCreateBtn
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets16916)
-         at ActivityPageanonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets8715)
-         at fulfilled
-      (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets558)
- </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> edit endDate of activity
-   1) AssertionError expected false to deeply equal true
-      + expected - actual
-      -false
-      +true
-      Browser Chrome 9204515159  Windows 10
-         175 áááá   checking if activity title exists
-         176   returns null
-         177 
-         178 async pressCreateBtn() 
-         179   await t
-        180     expect(thiscreateBtnexists)eql(true)
-         181     click(thiscreateBtn)
-         182     wait(2000)
-         183     expect(Selector(activityTitle)exists)
-         184     eql(true)
-         185   return null
-         at ActivityPageanonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets18037)
-         at anonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets871)
-         at __awaiter
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets412)
-         at ActivityPagepressCreateBtn
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets16916)
-         at ActivityPageanonymous
-   (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets8715)
-         at fulfilled
-      (CUsersmmfulDesktop9-9-21-anarkSVVSD-Test-CafematthewfullerPageObjectsactivity-pagets558)
+ Log in to MBEweb
 </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> can navigate to edit activity
-   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> can create an activity
-   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> can create an activity with multiple groups
-   </t>
   </si>
   <si>
     <t xml:space="preserve"> cannot create an activity without a title or desc
@@ -284,15 +178,11 @@
    </t>
   </si>
   <si>
-    <t xml:space="preserve"> edit title of activity
+    <t xml:space="preserve"> edit endDate of activity
    </t>
   </si>
   <si>
-    <t xml:space="preserve"> edit description of activity
-   </t>
-  </si>
-  <si>
-    <t xml:space="preserve"> edit endDate of activity
+    <t xml:space="preserve"> edit startDate of activity
    </t>
   </si>
 </sst>
@@ -628,7 +518,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A2"/>
+  <dimension ref="A1:A7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -644,6 +534,31 @@
         <v>2</v>
       </c>
     </row>
+    <row r="3" spans="1:1">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -651,7 +566,7 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A2:B9"/>
+  <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -661,68 +576,36 @@
     <col min="2" max="3" width="150.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="1364" customHeight="1">
+    <row r="2" spans="1:2" ht="1030" customHeight="1">
       <c r="A2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" ht="1464" customHeight="1">
+      <c r="A3" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" ht="1386" customHeight="1">
+      <c r="A4" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" ht="996" customHeight="1">
+      <c r="A5" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>11</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" ht="979" customHeight="1">
-      <c r="A3" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" ht="1039" customHeight="1">
-      <c r="A4" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" ht="1023" customHeight="1">
-      <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" ht="1023" customHeight="1">
-      <c r="A6" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" ht="1357" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" ht="1363" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" ht="1358" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -732,7 +615,7 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:A9"/>
+  <dimension ref="A1:A5"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
@@ -748,42 +631,22 @@
     </row>
     <row r="2" spans="1:1" ht="20" customHeight="1">
       <c r="A2" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="20" customHeight="1">
       <c r="A3" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="20" customHeight="1">
       <c r="A4" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="20" customHeight="1">
       <c r="A5" s="1" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" ht="20" customHeight="1">
-      <c r="A6" s="1" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" ht="20" customHeight="1">
-      <c r="A7" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="8" spans="1:1" ht="20" customHeight="1">
-      <c r="A8" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="9" spans="1:1" ht="20" customHeight="1">
-      <c r="A9" s="1" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
activite tests fully fixed and sorted
</commit_message>
<xml_diff>
--- a/matthew.fuller/results.xlsx
+++ b/matthew.fuller/results.xlsx
@@ -1,17 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24701"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/13a5b47c0ecfc38d/inportant_docs/school/annark/SVVSD-Test-Cafe/matthew.fuller/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_33E2DDEAF9F22574D3F67714993E2BBB3E8F8EBB" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{5DCC98D8-85FE-4953-8CC3-47EFD4711B0C}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="succsesses" sheetId="1" r:id="rId1"/>
     <sheet name="failsAndErrors" sheetId="2" r:id="rId2"/>
     <sheet name="fails" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
@@ -189,8 +195,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -230,6 +236,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -276,7 +290,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -308,9 +322,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -342,6 +374,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -517,44 +567,49 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:A7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="68" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" ht="255" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:1">
+    <row r="2" spans="1:1" ht="240" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:1">
+    <row r="3" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:1">
+    <row r="4" spans="1:1" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:1">
+    <row r="5" spans="1:1" ht="120" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="6" spans="1:1">
+    <row r="6" spans="1:1" ht="75" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="7" spans="1:1">
+    <row r="7" spans="1:1" ht="90" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
         <v>7</v>
       </c>
@@ -565,18 +620,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A2:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.7109375" customWidth="1"/>
     <col min="2" max="3" width="150.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:2" ht="1030" customHeight="1">
+    <row r="2" spans="1:2" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
@@ -584,7 +641,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:2" ht="1464" customHeight="1">
+    <row r="3" spans="1:2" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
@@ -592,7 +649,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:2" ht="1386" customHeight="1">
+    <row r="4" spans="1:2" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
@@ -600,7 +657,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:2" ht="996" customHeight="1">
+    <row r="5" spans="1:2" ht="409.6" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>
@@ -614,37 +671,39 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="70.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="20" customHeight="1">
+    <row r="2" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:1" ht="20" customHeight="1">
+    <row r="3" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:1" ht="20" customHeight="1">
+    <row r="4" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="5" spans="1:1" ht="20" customHeight="1">
+    <row r="5" spans="1:1" ht="20.100000000000001" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
         <v>15</v>
       </c>

</xml_diff>